<commit_message>
Capex and opex battery storge has been fixed. Now, it can simulate different scenarios by changing capex and opex from battery
</commit_message>
<xml_diff>
--- a/excel_file/LCOH_2030-Storage.xlsx
+++ b/excel_file/LCOH_2030-Storage.xlsx
@@ -439,7 +439,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="22.8" customWidth="1" min="1" max="1"/>
-    <col width="8.4" customWidth="1" min="2" max="2"/>
+    <col width="9.6" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -461,7 +461,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>4.46</v>
+        <v>132.04</v>
       </c>
     </row>
     <row r="3">
@@ -471,7 +471,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>14.13</v>
+        <v>563.3</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>3.27</v>
+        <v>58.67</v>
       </c>
     </row>
     <row r="5">
@@ -501,7 +501,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>4.19</v>
+        <v>139.11</v>
       </c>
     </row>
     <row r="7">
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>14.41</v>
+        <v>595.17</v>
       </c>
     </row>
     <row r="8">
@@ -521,7 +521,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>2.93</v>
+        <v>61.52</v>
       </c>
     </row>
     <row r="9">
@@ -541,7 +541,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>8.449999999999999</v>
+        <v>107.99</v>
       </c>
     </row>
     <row r="11">
@@ -551,7 +551,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>15.99</v>
+        <v>444.46</v>
       </c>
     </row>
     <row r="12">
@@ -561,7 +561,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>7.52</v>
+        <v>50.75</v>
       </c>
     </row>
     <row r="13">
@@ -581,7 +581,7 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>5.6</v>
+        <v>128.01</v>
       </c>
     </row>
     <row r="15">
@@ -591,7 +591,7 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>14.87</v>
+        <v>541.8</v>
       </c>
     </row>
     <row r="16">
@@ -601,7 +601,7 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>4.45</v>
+        <v>57.61</v>
       </c>
     </row>
     <row r="17">
@@ -656,7 +656,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>5.75</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="3">
@@ -666,7 +666,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>5.98</v>
+        <v>6.04</v>
       </c>
     </row>
     <row r="4">
@@ -676,7 +676,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>6.32</v>
+        <v>6.37</v>
       </c>
     </row>
     <row r="5">
@@ -696,7 +696,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>5.55</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="7">
@@ -706,7 +706,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>5.79</v>
+        <v>5.87</v>
       </c>
     </row>
     <row r="8">
@@ -716,7 +716,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>6.16</v>
+        <v>6.21</v>
       </c>
     </row>
     <row r="9">
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>9.449999999999999</v>
+        <v>9.56</v>
       </c>
     </row>
     <row r="11">
@@ -746,7 +746,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>9.630000000000001</v>
+        <v>9.69</v>
       </c>
     </row>
     <row r="12">
@@ -756,7 +756,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>9.9</v>
+        <v>9.94</v>
       </c>
     </row>
     <row r="13">
@@ -776,7 +776,7 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>6.83</v>
+        <v>6.96</v>
       </c>
     </row>
     <row r="15">
@@ -786,7 +786,7 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>7.05</v>
+        <v>7.12</v>
       </c>
     </row>
     <row r="16">
@@ -796,7 +796,7 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>7.38</v>
+        <v>7.43</v>
       </c>
     </row>
     <row r="17">
@@ -829,7 +829,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="22.8" customWidth="1" min="1" max="1"/>
-    <col width="8.4" customWidth="1" min="2" max="2"/>
+    <col width="9.6" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -851,7 +851,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>18.62</v>
+        <v>146.2</v>
       </c>
     </row>
     <row r="3">
@@ -861,7 +861,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>14.52</v>
+        <v>73.36</v>
       </c>
     </row>
     <row r="4">
@@ -871,7 +871,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>36.83</v>
+        <v>92.23</v>
       </c>
     </row>
     <row r="5">
@@ -891,7 +891,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>19.16</v>
+        <v>154.08</v>
       </c>
     </row>
     <row r="7">
@@ -901,7 +901,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>14.83</v>
+        <v>77.05</v>
       </c>
     </row>
     <row r="8">
@@ -911,7 +911,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>38.42</v>
+        <v>97.01000000000001</v>
       </c>
     </row>
     <row r="9">
@@ -931,7 +931,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>19.49</v>
+        <v>119.03</v>
       </c>
     </row>
     <row r="11">
@@ -941,7 +941,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>16.3</v>
+        <v>62.2</v>
       </c>
     </row>
     <row r="12">
@@ -951,7 +951,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>33.7</v>
+        <v>76.93000000000001</v>
       </c>
     </row>
     <row r="13">
@@ -971,7 +971,7 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>19.18</v>
+        <v>141.59</v>
       </c>
     </row>
     <row r="15">
@@ -981,7 +981,7 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>15.25</v>
+        <v>71.7</v>
       </c>
     </row>
     <row r="16">
@@ -991,7 +991,7 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>36.65</v>
+        <v>89.81</v>
       </c>
     </row>
     <row r="17">

</xml_diff>

<commit_message>
Variables representing conservative present scenario have been inserted. However, it still need to consider capacity factor for renewable sourcers. The selected capacity factors were only choosen to analyze the code behavior
</commit_message>
<xml_diff>
--- a/excel_file/LCOH_2030-Storage.xlsx
+++ b/excel_file/LCOH_2030-Storage.xlsx
@@ -439,7 +439,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="22.8" customWidth="1" min="1" max="1"/>
-    <col width="9.6" customWidth="1" min="2" max="2"/>
+    <col width="8.4" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -461,7 +461,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>132.04</v>
+        <v>7.71</v>
       </c>
     </row>
     <row r="3">
@@ -471,7 +471,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>563.3</v>
+        <v>5.53</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>58.67</v>
+        <v>8.33</v>
       </c>
     </row>
     <row r="5">
@@ -491,7 +491,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>1.85</v>
+        <v>8.24</v>
       </c>
     </row>
     <row r="6">
@@ -501,7 +501,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>139.11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>595.17</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="8">
@@ -521,7 +521,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>61.52</v>
+        <v>7.66</v>
       </c>
     </row>
     <row r="9">
@@ -531,7 +531,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>1.43</v>
+        <v>7.56</v>
       </c>
     </row>
     <row r="10">
@@ -541,7 +541,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>107.99</v>
+        <v>15.8</v>
       </c>
     </row>
     <row r="11">
@@ -551,7 +551,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>444.46</v>
+        <v>14.11</v>
       </c>
     </row>
     <row r="12">
@@ -561,7 +561,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>50.75</v>
+        <v>16.29</v>
       </c>
     </row>
     <row r="13">
@@ -571,7 +571,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>6.42</v>
+        <v>16.22</v>
       </c>
     </row>
     <row r="14">
@@ -581,7 +581,7 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>128.01</v>
+        <v>7.95</v>
       </c>
     </row>
     <row r="15">
@@ -591,7 +591,7 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>541.8</v>
+        <v>5.86</v>
       </c>
     </row>
     <row r="16">
@@ -601,7 +601,7 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>57.61</v>
+        <v>8.539999999999999</v>
       </c>
     </row>
     <row r="17">
@@ -611,7 +611,7 @@
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>3.09</v>
+        <v>8.449999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -666,7 +666,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>6.04</v>
+        <v>4.41</v>
       </c>
     </row>
     <row r="4">
@@ -706,7 +706,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>5.87</v>
+        <v>4.14</v>
       </c>
     </row>
     <row r="8">
@@ -746,7 +746,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>9.69</v>
+        <v>8.41</v>
       </c>
     </row>
     <row r="12">
@@ -786,7 +786,7 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>7.12</v>
+        <v>5.55</v>
       </c>
     </row>
     <row r="16">
@@ -861,7 +861,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>73.36</v>
+        <v>68.48999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -901,7 +901,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>77.05</v>
+        <v>71.90000000000001</v>
       </c>
     </row>
     <row r="8">
@@ -941,7 +941,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>62.2</v>
+        <v>58.41</v>
       </c>
     </row>
     <row r="12">
@@ -981,7 +981,7 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>71.7</v>
+        <v>67.03</v>
       </c>
     </row>
     <row r="16">

</xml_diff>

<commit_message>
The 2025 data for renewable energies and electrolyzers for various scenarios  has been inserted
</commit_message>
<xml_diff>
--- a/excel_file/LCOH_2030-Storage.xlsx
+++ b/excel_file/LCOH_2030-Storage.xlsx
@@ -461,7 +461,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>7.71</v>
+        <v>10.03</v>
       </c>
     </row>
     <row r="3">
@@ -471,7 +471,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>5.53</v>
+        <v>5.08</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>8.33</v>
+        <v>6.91</v>
       </c>
     </row>
     <row r="5">
@@ -491,7 +491,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>8.24</v>
+        <v>5.46</v>
       </c>
     </row>
     <row r="6">
@@ -501,7 +501,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>7</v>
+        <v>9.460000000000001</v>
       </c>
     </row>
     <row r="7">
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>4.7</v>
+        <v>4.22</v>
       </c>
     </row>
     <row r="8">
@@ -521,7 +521,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>7.66</v>
+        <v>6.16</v>
       </c>
     </row>
     <row r="9">
@@ -531,7 +531,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>7.56</v>
+        <v>4.63</v>
       </c>
     </row>
     <row r="10">
@@ -541,7 +541,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>15.8</v>
+        <v>17.62</v>
       </c>
     </row>
     <row r="11">
@@ -551,7 +551,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>14.11</v>
+        <v>13.75</v>
       </c>
     </row>
     <row r="12">
@@ -561,7 +561,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>16.29</v>
+        <v>15.18</v>
       </c>
     </row>
     <row r="13">
@@ -571,7 +571,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>16.22</v>
+        <v>14.05</v>
       </c>
     </row>
     <row r="14">
@@ -581,7 +581,7 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>7.95</v>
+        <v>10.18</v>
       </c>
     </row>
     <row r="15">
@@ -591,7 +591,7 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>5.86</v>
+        <v>5.42</v>
       </c>
     </row>
     <row r="16">
@@ -601,7 +601,7 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>8.539999999999999</v>
+        <v>7.18</v>
       </c>
     </row>
     <row r="17">
@@ -611,7 +611,7 @@
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>8.449999999999999</v>
+        <v>5.79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>